<commit_message>
add lab2 and 3
</commit_message>
<xml_diff>
--- a/lab2/Lab02_Review Report.xlsx
+++ b/lab2/Lab02_Review Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaimarianionut/Documents/GitHub/vvta2021/lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED33EB2-10D4-9E4D-AE26-7C2C52B43FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ABE63C-13C2-E64F-A0C1-9F6EC8733C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10300" yWindow="1960" windowWidth="18800" windowHeight="14860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="2420" windowWidth="22260" windowHeight="14860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -117,27 +117,18 @@
     <t>Mihai Ionut</t>
   </si>
   <si>
-    <t>I01</t>
-  </si>
-  <si>
     <t>CerinteAngajati-Initial.pdf.1/i</t>
   </si>
   <si>
     <t xml:space="preserve">Sa se adauge si departamentul </t>
   </si>
   <si>
-    <t>I02</t>
-  </si>
-  <si>
     <t>CerinteAngajati-Initial.pdf.1/iii</t>
   </si>
   <si>
     <t>Sa se adauge anul nasterii</t>
   </si>
   <si>
-    <t>I03</t>
-  </si>
-  <si>
     <t>Nu se specifica date cu privire la initializarea sistemului</t>
   </si>
   <si>
@@ -150,15 +141,9 @@
     <t>Modificarea mai multor date, cnp, salariu, nume, prenume</t>
   </si>
   <si>
-    <t>I04</t>
-  </si>
-  <si>
     <t>Ordinea crescatoare trebuie facuta dupa varsta calculata din anul nasterii, nu din cnp .</t>
   </si>
   <si>
-    <t>IO1</t>
-  </si>
-  <si>
     <t>DiagramaSalariati-Initial.png/ EmployeeImpl</t>
   </si>
   <si>
@@ -183,9 +168,6 @@
     <t>Trebuie adaugat un nou layer la arhitectura, si anume layer-ul service</t>
   </si>
   <si>
-    <t>IO4</t>
-  </si>
-  <si>
     <t>Crearea unui pachet nou pentru exceptii</t>
   </si>
   <si>
@@ -198,9 +180,6 @@
     <t>Trebuie redenumita pentru nu a exista confuzi u clasele de test</t>
   </si>
   <si>
-    <t>IO6</t>
-  </si>
-  <si>
     <t>Nu se specifica proprietati de agregare sau compozitie intr-e clase</t>
   </si>
   <si>
@@ -307,6 +286,45 @@
   </si>
   <si>
     <t>Nested try catch</t>
+  </si>
+  <si>
+    <t>AO6</t>
+  </si>
+  <si>
+    <t>AO1</t>
+  </si>
+  <si>
+    <t>AO1,AO8</t>
+  </si>
+  <si>
+    <t>AO1,AO7</t>
+  </si>
+  <si>
+    <t>AO9</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>RO1</t>
+  </si>
+  <si>
+    <t>RO7</t>
+  </si>
+  <si>
+    <t>RO4</t>
+  </si>
+  <si>
+    <t>RO7,06</t>
+  </si>
+  <si>
+    <t>Unused field</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -890,8 +908,8 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -975,13 +993,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -990,13 +1008,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1005,13 +1023,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1020,13 +1038,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1035,13 +1053,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1175,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1260,13 +1278,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -1275,13 +1293,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1290,13 +1308,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1305,13 +1323,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1320,13 +1338,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1335,13 +1353,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1475,8 +1493,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1560,13 +1578,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1575,13 +1593,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1590,13 +1608,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1605,13 +1623,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1620,13 +1638,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1635,13 +1653,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1650,13 +1668,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -1665,13 +1683,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -1800,7 +1818,7 @@
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1823,8 +1841,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1899,16 +1917,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1917,16 +1935,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1935,16 +1953,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1953,27 +1971,35 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="20">

</xml_diff>